<commit_message>
added initial support for puckjs
</commit_message>
<xml_diff>
--- a/documentation/Map.xlsx
+++ b/documentation/Map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="125">
   <si>
     <t>ID</t>
   </si>
@@ -304,9 +304,6 @@
     <t>PKi</t>
   </si>
   <si>
-    <t>PBa</t>
-  </si>
-  <si>
     <t>PHa</t>
   </si>
   <si>
@@ -395,6 +392,9 @@
   </si>
   <si>
     <t>Meter_Water_Warm</t>
+  </si>
+  <si>
+    <t>PB</t>
   </si>
 </sst>
 </file>
@@ -425,15 +425,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -441,11 +447,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -455,6 +472,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1315,7 +1334,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>1</a:t>
+            <a:t>0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1375,6 +1394,66 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>25212</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>173131</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>4212</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152131</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Ellipse 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4686859" y="2459131"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:t>2</a:t>
           </a:r>
         </a:p>
@@ -1384,25 +1463,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>36418</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>72278</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38660</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>174813</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>15418</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>51278</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>17660</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>153813</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Ellipse 19"/>
+        <xdr:cNvPr id="21" name="Ellipse 20"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4698065" y="2358278"/>
+          <a:off x="2414307" y="746313"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1444,25 +1523,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>94689</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>129989</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>148477</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>186578</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>73689</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>108989</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>127477</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165578</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Ellipse 20"/>
+        <xdr:cNvPr id="22" name="Ellipse 21"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2470336" y="701489"/>
+          <a:off x="3857624" y="2853578"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1504,25 +1583,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>25212</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>108137</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>186015</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>4212</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>87137</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>165015</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Ellipse 21"/>
+        <xdr:cNvPr id="23" name="Ellipse 22"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4686859" y="2965637"/>
+          <a:off x="4276162" y="0"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1565,24 +1644,24 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>40340</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>25213</xdr:rowOff>
+      <xdr:colOff>24092</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>174251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>19340</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>4213</xdr:rowOff>
+      <xdr:colOff>3092</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>153251</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Ellipse 22"/>
+        <xdr:cNvPr id="24" name="Ellipse 23"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4701987" y="25213"/>
+          <a:off x="4685739" y="1698251"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1624,45 +1703,42 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>35298</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>6163</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>100856</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>164165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>14298</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>175663</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>79856</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>143165</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Ellipse 23"/>
+        <xdr:cNvPr id="26" name="Ellipse 25"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4696945" y="2673163"/>
+          <a:off x="3429003" y="3783665"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FF0000"/>
-        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="accent2">
             <a:shade val="50000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent2"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -1675,7 +1751,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>7</a:t>
+            <a:t>0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1684,25 +1760,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>127747</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>101412</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>17930</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>106747</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>80412</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>187430</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Ellipse 24"/>
+        <xdr:cNvPr id="27" name="Ellipse 26"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4408394" y="2958912"/>
+          <a:off x="3917577" y="0"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1733,120 +1809,6 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:t>2</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>67238</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>7283</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>46238</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>176783</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Ellipse 25"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3585885" y="3817283"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>163608</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>142608</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1412</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="Ellipse 26"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4444255" y="22412"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>3</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1903,6 +1865,63 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>0</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>40341</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>170892</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>19341</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>149892</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Ellipse 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4320988" y="2456892"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:t>1</a:t>
           </a:r>
         </a:p>
@@ -1912,25 +1931,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>85165</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>36421</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47064</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>64165</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>15421</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>26064</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>179026</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="Ellipse 28"/>
+        <xdr:cNvPr id="30" name="Ellipse 29"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4365812" y="2322421"/>
+          <a:off x="2422711" y="390526"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1969,25 +1988,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>125505</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>76761</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>17927</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>182098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>104505</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>55761</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>187427</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161098</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="Ellipse 29"/>
+        <xdr:cNvPr id="31" name="Ellipse 30"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2501152" y="457761"/>
+          <a:off x="4679574" y="2087098"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1996,15 +2015,15 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent5">
+          <a:schemeClr val="accent4">
             <a:shade val="50000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent5"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -2017,7 +2036,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>3</a:t>
+            <a:t>0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2026,25 +2045,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>107574</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>182098</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>170328</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>166409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>86574</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161098</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>149328</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>145409</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="Ellipse 30"/>
+        <xdr:cNvPr id="32" name="Ellipse 31"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4388221" y="2658598"/>
+          <a:off x="4641475" y="356909"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2083,25 +2102,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>91886</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>76762</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>70886</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>55762</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>179028</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="Ellipse 31"/>
+        <xdr:cNvPr id="33" name="Ellipse 32"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4182033" y="267262"/>
+          <a:off x="3420033" y="3438528"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2110,15 +2129,15 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent4">
+          <a:schemeClr val="accent3">
             <a:shade val="50000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent4"/>
+          <a:schemeClr val="accent3"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
+          <a:schemeClr val="accent3"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -2131,7 +2150,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>2</a:t>
+            <a:t>0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2140,25 +2159,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>2239</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9527</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>154637</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>5043</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>171739</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>179027</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>133637</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>174543</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="Ellipse 32"/>
+        <xdr:cNvPr id="34" name="Ellipse 33"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3330386" y="3819527"/>
+          <a:off x="5006784" y="5043"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2197,73 +2216,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>165845</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>94691</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>170328</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>144845</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>73691</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="Ellipse 33"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4446492" y="285191"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>2</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>91886</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>20731</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>70886</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>149328</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>190231</xdr:rowOff>
+      <xdr:rowOff>169500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2272,7 +2234,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4182033" y="20731"/>
+          <a:off x="4641475" y="0"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2305,7 +2267,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>8</a:t>
+            <a:t>7</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2374,16 +2336,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>561</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>168649</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>17099</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>170061</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>147649</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2392,7 +2354,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4128246" y="2477061"/>
+          <a:off x="4318746" y="2073649"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2400,6 +2362,192 @@
         </a:prstGeom>
         <a:solidFill>
           <a:srgbClr val="42BA06"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>0</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>126065</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>105065</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>46235</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Ellipse 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1358712" y="67235"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>0</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>166406</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>163605</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>145406</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142605</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Ellipse 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2923053" y="6640605"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>25211</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>4211</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Ellipse 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3924858" y="381000"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -2434,25 +2582,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>114859</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>81243</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>93859</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>23824</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>60243</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>102263</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="Ellipse 37"/>
+        <xdr:cNvPr id="42" name="Ellipse 41"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2300006" y="44824"/>
+          <a:off x="1885390" y="3742763"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2496,264 +2644,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>29135</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>179024</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>8135</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="Ellipse 38"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2956671" y="6315635"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>25212</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>134470</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>4212</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>113470</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="Ellipse 39"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4686859" y="1277470"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>3</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>182094</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:colOff>96371</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>161094</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>147088</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="Ellipse 40"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1414741" y="2454088"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>4</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>25213</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>89646</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>4213</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>68646</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="Ellipse 41"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3353360" y="3518646"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>5</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>29136</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>103653</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>8136</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>82653</xdr:rowOff>
+      <xdr:colOff>75371</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>172300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2762,7 +2662,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1833283" y="1056153"/>
+          <a:off x="1329018" y="955300"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2808,16 +2708,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>147919</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>87965</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>24654</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>54347</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>126919</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>66965</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3654</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>33347</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2826,7 +2726,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2333066" y="3516965"/>
+          <a:off x="2590801" y="3292847"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2868,16 +2768,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>4482</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>135032</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>183776</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>157444</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>173982</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>114032</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>162776</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>136444</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2886,7 +2786,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2951629" y="6040532"/>
+          <a:off x="2559423" y="6634444"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2928,25 +2828,145 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>168088</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>163606</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>81243</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>147088</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>53520</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142606</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60243</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="Ellipse 45"/>
+        <xdr:cNvPr id="47" name="Ellipse 46"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1400735" y="2741520"/>
+          <a:off x="1015253" y="81243"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="42BA06"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>58271</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>188820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>37271</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>167820</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Ellipse 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3576918" y="379320"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="42BA06"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>4</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>109817</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>117101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>88817</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>96101</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Ellipse 48"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1532964" y="3736601"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2989,24 +3009,24 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>62753</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>58831</xdr:rowOff>
+      <xdr:colOff>71717</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>41753</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>37831</xdr:rowOff>
+      <xdr:colOff>50717</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>158294</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="Ellipse 46"/>
+        <xdr:cNvPr id="50" name="Ellipse 49"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2057400" y="58831"/>
+          <a:off x="2066364" y="4751294"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3039,7 +3059,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>3</a:t>
+            <a:t>1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3048,196 +3068,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>35859</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>42583</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>184336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>14859</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>179026</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="Ellipse 47"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4697506" y="962026"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="42BA06"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>4</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>87406</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>94690</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>66406</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>73690</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="Ellipse 48"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3606053" y="3523690"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="42BA06"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>6</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>105334</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>84334</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>169500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Ellipse 49"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3242981" y="0"/>
-          <a:ext cx="360000" cy="360000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="42BA06"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" b="1"/>
-            <a:t>A</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>31377</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>139512</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>10377</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>118512</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>21583</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>163336</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3246,7 +3086,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4121524" y="2806512"/>
+          <a:off x="3942230" y="2089336"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3289,15 +3129,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>181536</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>99171</xdr:rowOff>
+      <xdr:colOff>125505</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>166407</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>160536</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>78171</xdr:rowOff>
+      <xdr:colOff>104505</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>145407</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3306,7 +3146,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1414183" y="1051671"/>
+          <a:off x="1358152" y="547407"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3467,15 +3307,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>100853</xdr:colOff>
+      <xdr:colOff>89647</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>123264</xdr:rowOff>
+      <xdr:rowOff>123263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>79853</xdr:colOff>
+      <xdr:colOff>68647</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>102264</xdr:rowOff>
+      <xdr:rowOff>102263</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3484,7 +3324,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4381500" y="6600264"/>
+          <a:off x="4370294" y="6600263"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3529,13 +3369,13 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>118782</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>118782</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>97782</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>97782</xdr:rowOff>
+      <xdr:rowOff>131399</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3544,7 +3384,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3446929" y="6595782"/>
+          <a:off x="3446929" y="6629399"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3587,15 +3427,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>69476</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>35858</xdr:rowOff>
+      <xdr:rowOff>47064</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>93300</xdr:colOff>
+      <xdr:colOff>48476</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>14858</xdr:rowOff>
+      <xdr:rowOff>26064</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3604,7 +3444,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1727947" y="2893358"/>
+          <a:off x="1683123" y="2904564"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3706,16 +3546,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>105335</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>105335</xdr:rowOff>
+      <xdr:rowOff>60511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>84335</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>17100</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>84335</xdr:rowOff>
+      <xdr:rowOff>39511</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3724,7 +3564,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1718982" y="105335"/>
+          <a:off x="1842247" y="60511"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3769,13 +3609,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>168088</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
+      <xdr:rowOff>168089</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>147088</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>23824</xdr:rowOff>
+      <xdr:rowOff>147089</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3784,7 +3624,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1400735" y="2140324"/>
+          <a:off x="1400735" y="2263589"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3827,15 +3667,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>96370</xdr:colOff>
+      <xdr:colOff>73958</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>51548</xdr:rowOff>
+      <xdr:rowOff>107578</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>75370</xdr:colOff>
+      <xdr:colOff>52958</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>30548</xdr:rowOff>
+      <xdr:rowOff>86578</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3844,7 +3684,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1900517" y="3290048"/>
+          <a:off x="1878105" y="3346078"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3889,13 +3729,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>163605</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>96372</xdr:rowOff>
+      <xdr:rowOff>186019</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>142605</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>75372</xdr:rowOff>
+      <xdr:rowOff>165019</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3904,7 +3744,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1396252" y="1810872"/>
+          <a:off x="1396252" y="1900519"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3938,6 +3778,63 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:t>0</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>17931</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>170889</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>187431</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>149889</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Ellipse 67"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4679578" y="2837889"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4230,8 +4127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK38" sqref="AK38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4281,7 +4178,7 @@
         <v>54</v>
       </c>
       <c r="AP1" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="28:42" x14ac:dyDescent="0.25">
@@ -4295,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="AI2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ2">
         <v>0</v>
@@ -4316,7 +4213,7 @@
         <v>19</v>
       </c>
       <c r="AP2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="28:42" x14ac:dyDescent="0.25">
@@ -4327,7 +4224,7 @@
         <v>1</v>
       </c>
       <c r="AI3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ3">
         <v>1</v>
@@ -4348,7 +4245,7 @@
         <v>19</v>
       </c>
       <c r="AP3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="28:42" x14ac:dyDescent="0.25">
@@ -4362,16 +4259,16 @@
         <v>2</v>
       </c>
       <c r="AI4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ4">
         <v>2</v>
       </c>
       <c r="AK4">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AL4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AM4" t="s">
         <v>21</v>
@@ -4383,7 +4280,7 @@
         <v>22</v>
       </c>
       <c r="AP4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="28:42" x14ac:dyDescent="0.25">
@@ -4394,7 +4291,7 @@
         <v>3</v>
       </c>
       <c r="AI5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ5">
         <v>3</v>
@@ -4415,7 +4312,7 @@
         <v>24</v>
       </c>
       <c r="AP5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="28:42" x14ac:dyDescent="0.25">
@@ -4429,7 +4326,7 @@
         <v>4</v>
       </c>
       <c r="AI6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ6">
         <v>4</v>
@@ -4438,7 +4335,7 @@
         <v>55</v>
       </c>
       <c r="AL6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AM6" t="s">
         <v>25</v>
@@ -4450,7 +4347,7 @@
         <v>22</v>
       </c>
       <c r="AP6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="28:42" x14ac:dyDescent="0.25">
@@ -4461,7 +4358,7 @@
         <v>5</v>
       </c>
       <c r="AI7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ7">
         <v>5</v>
@@ -4470,7 +4367,7 @@
         <v>99</v>
       </c>
       <c r="AL7">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="AM7" t="s">
         <v>26</v>
@@ -4482,7 +4379,7 @@
         <v>22</v>
       </c>
       <c r="AP7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="28:42" x14ac:dyDescent="0.25">
@@ -4496,16 +4393,16 @@
         <v>6</v>
       </c>
       <c r="AI8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ8">
         <v>6</v>
       </c>
       <c r="AK8">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="AL8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AM8" t="s">
         <v>27</v>
@@ -4517,7 +4414,7 @@
         <v>22</v>
       </c>
       <c r="AP8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="28:42" x14ac:dyDescent="0.25">
@@ -4528,7 +4425,7 @@
         <v>7</v>
       </c>
       <c r="AI9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ9">
         <v>7</v>
@@ -4537,7 +4434,7 @@
         <v>99</v>
       </c>
       <c r="AL9">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AM9" t="s">
         <v>52</v>
@@ -4549,7 +4446,7 @@
         <v>22</v>
       </c>
       <c r="AP9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="28:42" x14ac:dyDescent="0.25">
@@ -4572,7 +4469,7 @@
         <v>43</v>
       </c>
       <c r="AL10">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="AM10" t="s">
         <v>46</v>
@@ -4584,7 +4481,7 @@
         <v>56</v>
       </c>
       <c r="AP10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="28:42" x14ac:dyDescent="0.25">
@@ -4601,10 +4498,10 @@
         <v>1</v>
       </c>
       <c r="AK11">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AL11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AM11" t="s">
         <v>47</v>
@@ -4616,7 +4513,7 @@
         <v>22</v>
       </c>
       <c r="AP11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="28:42" x14ac:dyDescent="0.25">
@@ -4626,8 +4523,8 @@
       <c r="AF12" t="s">
         <v>33</v>
       </c>
-      <c r="AH12" t="s">
-        <v>107</v>
+      <c r="AH12">
+        <v>10</v>
       </c>
       <c r="AI12" t="s">
         <v>29</v>
@@ -4639,7 +4536,7 @@
         <v>99</v>
       </c>
       <c r="AL12">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="AM12" t="s">
         <v>48</v>
@@ -4651,7 +4548,7 @@
         <v>22</v>
       </c>
       <c r="AP12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="28:42" x14ac:dyDescent="0.25">
@@ -4659,7 +4556,7 @@
         <v>65</v>
       </c>
       <c r="AH13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AI13" t="s">
         <v>30</v>
@@ -4683,7 +4580,7 @@
         <v>19</v>
       </c>
       <c r="AP13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="28:42" x14ac:dyDescent="0.25">
@@ -4694,7 +4591,7 @@
         <v>34</v>
       </c>
       <c r="AH14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AI14" t="s">
         <v>30</v>
@@ -4703,10 +4600,10 @@
         <v>1</v>
       </c>
       <c r="AK14">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AL14">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AM14" t="s">
         <v>21</v>
@@ -4718,7 +4615,7 @@
         <v>22</v>
       </c>
       <c r="AP14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="28:42" x14ac:dyDescent="0.25">
@@ -4726,7 +4623,7 @@
         <v>60</v>
       </c>
       <c r="AH15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AI15" t="s">
         <v>30</v>
@@ -4750,7 +4647,7 @@
         <v>24</v>
       </c>
       <c r="AP15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="28:42" x14ac:dyDescent="0.25">
@@ -4761,7 +4658,7 @@
         <v>35</v>
       </c>
       <c r="AH16">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AI16" t="s">
         <v>44</v>
@@ -4770,10 +4667,10 @@
         <v>0</v>
       </c>
       <c r="AK16">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="AL16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AM16" t="s">
         <v>51</v>
@@ -4785,7 +4682,7 @@
         <v>22</v>
       </c>
       <c r="AP16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="28:42" x14ac:dyDescent="0.25">
@@ -4793,7 +4690,7 @@
         <v>55</v>
       </c>
       <c r="AH17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AI17" t="s">
         <v>44</v>
@@ -4805,7 +4702,7 @@
         <v>94</v>
       </c>
       <c r="AL17">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AM17" t="s">
         <v>52</v>
@@ -4817,7 +4714,7 @@
         <v>22</v>
       </c>
       <c r="AP17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="28:42" x14ac:dyDescent="0.25">
@@ -4828,7 +4725,7 @@
         <v>36</v>
       </c>
       <c r="AH18">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AI18" t="s">
         <v>32</v>
@@ -4837,10 +4734,10 @@
         <v>0</v>
       </c>
       <c r="AK18">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="AL18">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AM18" t="s">
         <v>49</v>
@@ -4852,15 +4749,15 @@
         <v>56</v>
       </c>
       <c r="AP18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="28:42" x14ac:dyDescent="0.25">
       <c r="AB19">
         <v>50</v>
       </c>
-      <c r="AH19" t="s">
-        <v>107</v>
+      <c r="AH19">
+        <v>16</v>
       </c>
       <c r="AI19" t="s">
         <v>32</v>
@@ -4869,10 +4766,10 @@
         <v>1</v>
       </c>
       <c r="AK19">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="AL19">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AM19" t="s">
         <v>50</v>
@@ -4884,7 +4781,7 @@
         <v>22</v>
       </c>
       <c r="AP19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="28:42" x14ac:dyDescent="0.25">
@@ -4895,7 +4792,7 @@
         <v>37</v>
       </c>
       <c r="AH20">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AI20" t="s">
         <v>33</v>
@@ -4919,7 +4816,7 @@
         <v>56</v>
       </c>
       <c r="AP20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="28:42" x14ac:dyDescent="0.25">
@@ -4927,7 +4824,7 @@
         <v>45</v>
       </c>
       <c r="AH21">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AI21" t="s">
         <v>34</v>
@@ -4936,10 +4833,10 @@
         <v>0</v>
       </c>
       <c r="AK21">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AL21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AM21" t="s">
         <v>57</v>
@@ -4951,7 +4848,7 @@
         <v>22</v>
       </c>
       <c r="AP21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="28:42" x14ac:dyDescent="0.25">
@@ -4962,7 +4859,7 @@
         <v>38</v>
       </c>
       <c r="AH22">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AI22" t="s">
         <v>34</v>
@@ -4971,10 +4868,10 @@
         <v>1</v>
       </c>
       <c r="AK22">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="AL22">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="AM22" t="s">
         <v>68</v>
@@ -4986,15 +4883,15 @@
         <v>70</v>
       </c>
       <c r="AP22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="28:42" x14ac:dyDescent="0.25">
       <c r="AB23">
         <v>39</v>
       </c>
-      <c r="AH23" t="s">
-        <v>107</v>
+      <c r="AH23">
+        <v>20</v>
       </c>
       <c r="AI23" t="s">
         <v>34</v>
@@ -5003,10 +4900,10 @@
         <v>2</v>
       </c>
       <c r="AK23">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AL23">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AM23" t="s">
         <v>58</v>
@@ -5018,7 +4915,7 @@
         <v>19</v>
       </c>
       <c r="AP23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="28:42" x14ac:dyDescent="0.25">
@@ -5026,10 +4923,10 @@
         <v>36</v>
       </c>
       <c r="AF24" t="s">
-        <v>108</v>
-      </c>
-      <c r="AH24" t="s">
         <v>107</v>
+      </c>
+      <c r="AH24">
+        <v>21</v>
       </c>
       <c r="AI24" t="s">
         <v>34</v>
@@ -5041,7 +4938,7 @@
         <v>99</v>
       </c>
       <c r="AL24">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="AM24" t="s">
         <v>59</v>
@@ -5053,15 +4950,15 @@
         <v>24</v>
       </c>
       <c r="AP24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="28:42" x14ac:dyDescent="0.25">
       <c r="AB25">
         <v>33</v>
       </c>
-      <c r="AH25" t="s">
-        <v>107</v>
+      <c r="AH25">
+        <v>22</v>
       </c>
       <c r="AI25" t="s">
         <v>34</v>
@@ -5070,10 +4967,10 @@
         <v>4</v>
       </c>
       <c r="AK25">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="AL25">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="AM25" t="s">
         <v>60</v>
@@ -5085,15 +4982,15 @@
         <v>22</v>
       </c>
       <c r="AP25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="28:42" x14ac:dyDescent="0.25">
       <c r="AB26">
         <v>30</v>
       </c>
-      <c r="AH26" t="s">
-        <v>107</v>
+      <c r="AH26">
+        <v>23</v>
       </c>
       <c r="AI26" t="s">
         <v>34</v>
@@ -5102,22 +4999,22 @@
         <v>5</v>
       </c>
       <c r="AK26">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="AL26">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="AM26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AN26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AO26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AP26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="28:42" x14ac:dyDescent="0.25">
@@ -5125,7 +5022,7 @@
         <v>27</v>
       </c>
       <c r="AH27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AI27" t="s">
         <v>34</v>
@@ -5133,31 +5030,25 @@
       <c r="AJ27">
         <v>6</v>
       </c>
-      <c r="AK27">
-        <v>48</v>
-      </c>
-      <c r="AL27">
-        <v>30</v>
-      </c>
       <c r="AM27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AN27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AO27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AP27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="28:42" x14ac:dyDescent="0.25">
       <c r="AB28">
         <v>24</v>
       </c>
-      <c r="AH28" t="s">
-        <v>107</v>
+      <c r="AH28">
+        <v>24</v>
       </c>
       <c r="AI28" t="s">
         <v>35</v>
@@ -5166,30 +5057,30 @@
         <v>0</v>
       </c>
       <c r="AK28">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="AL28">
-        <v>40</v>
-      </c>
-      <c r="AM28" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN28" t="s">
-        <v>92</v>
-      </c>
-      <c r="AO28" t="s">
-        <v>19</v>
+        <v>75</v>
+      </c>
+      <c r="AM28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN28" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO28" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="AP28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="28:42" x14ac:dyDescent="0.25">
       <c r="AB29">
         <v>21</v>
       </c>
-      <c r="AH29" t="s">
-        <v>107</v>
+      <c r="AH29">
+        <v>25</v>
       </c>
       <c r="AI29" t="s">
         <v>35</v>
@@ -5198,30 +5089,30 @@
         <v>1</v>
       </c>
       <c r="AK29">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="AL29">
-        <v>58</v>
-      </c>
-      <c r="AM29" t="s">
-        <v>64</v>
-      </c>
-      <c r="AN29" t="s">
-        <v>93</v>
-      </c>
-      <c r="AO29" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="AM29" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO29" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="AP29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="28:42" x14ac:dyDescent="0.25">
       <c r="AB30">
         <v>18</v>
       </c>
-      <c r="AH30" t="s">
-        <v>107</v>
+      <c r="AH30">
+        <v>26</v>
       </c>
       <c r="AI30" t="s">
         <v>35</v>
@@ -5230,30 +5121,30 @@
         <v>2</v>
       </c>
       <c r="AK30">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="AL30">
-        <v>2</v>
-      </c>
-      <c r="AM30" t="s">
-        <v>65</v>
-      </c>
-      <c r="AN30" t="s">
-        <v>92</v>
-      </c>
-      <c r="AO30" t="s">
-        <v>22</v>
+        <v>63</v>
+      </c>
+      <c r="AM30" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO30" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="AP30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="28:42" x14ac:dyDescent="0.25">
       <c r="AB31">
         <v>15</v>
       </c>
-      <c r="AH31" t="s">
-        <v>107</v>
+      <c r="AH31">
+        <v>27</v>
       </c>
       <c r="AI31" t="s">
         <v>35</v>
@@ -5262,22 +5153,22 @@
         <v>3</v>
       </c>
       <c r="AK31">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="AL31">
-        <v>74</v>
-      </c>
-      <c r="AM31" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN31" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO31" t="s">
-        <v>55</v>
+        <v>43</v>
+      </c>
+      <c r="AM31" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN31" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO31" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="AP31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="28:42" x14ac:dyDescent="0.25">
@@ -5285,7 +5176,7 @@
         <v>12</v>
       </c>
       <c r="AH32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AI32" t="s">
         <v>35</v>
@@ -5293,23 +5184,17 @@
       <c r="AJ32">
         <v>4</v>
       </c>
-      <c r="AK32">
-        <v>48</v>
-      </c>
-      <c r="AL32">
-        <v>30</v>
-      </c>
       <c r="AM32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AN32" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="AO32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AP32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:42" x14ac:dyDescent="0.25">
@@ -5317,7 +5202,7 @@
         <v>10</v>
       </c>
       <c r="AH33">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="AI33" t="s">
         <v>36</v>
@@ -5326,22 +5211,22 @@
         <v>0</v>
       </c>
       <c r="AK33">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="AL33">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="AM33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AN33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AO33" t="s">
         <v>24</v>
       </c>
       <c r="AP33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:42" x14ac:dyDescent="0.25">
@@ -5349,7 +5234,7 @@
         <v>8</v>
       </c>
       <c r="AH34">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="AI34" t="s">
         <v>36</v>
@@ -5361,19 +5246,19 @@
         <v>83</v>
       </c>
       <c r="AL34">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AM34" t="s">
         <v>36</v>
       </c>
       <c r="AN34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AO34" t="s">
         <v>24</v>
       </c>
       <c r="AP34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:42" x14ac:dyDescent="0.25">
@@ -5381,7 +5266,7 @@
         <v>5</v>
       </c>
       <c r="AH35">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="AI35" t="s">
         <v>45</v>
@@ -5390,22 +5275,22 @@
         <v>0</v>
       </c>
       <c r="AK35">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="AL35">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="AM35" t="s">
         <v>45</v>
       </c>
       <c r="AN35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO35" t="s">
         <v>56</v>
       </c>
       <c r="AP35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:42" x14ac:dyDescent="0.25">
@@ -5413,7 +5298,7 @@
         <v>2</v>
       </c>
       <c r="AH36">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="AI36" t="s">
         <v>38</v>
@@ -5422,22 +5307,22 @@
         <v>0</v>
       </c>
       <c r="AK36">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="AL36">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AM36" t="s">
         <v>69</v>
       </c>
       <c r="AN36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO36" t="s">
         <v>22</v>
       </c>
       <c r="AP36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:42" x14ac:dyDescent="0.25">
@@ -5445,34 +5330,34 @@
         <v>0</v>
       </c>
       <c r="AC37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AH37">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ37">
         <v>0</v>
       </c>
       <c r="AK37">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AL37">
         <v>74</v>
       </c>
       <c r="AM37" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN37" t="s">
         <v>121</v>
-      </c>
-      <c r="AN37" t="s">
-        <v>122</v>
       </c>
       <c r="AO37" t="s">
         <v>55</v>
       </c>
       <c r="AP37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:42" x14ac:dyDescent="0.25">
@@ -5558,42 +5443,42 @@
         <v>0</v>
       </c>
       <c r="AH38">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="AI38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ38">
         <v>1</v>
       </c>
       <c r="AK38">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AL38">
         <v>74</v>
       </c>
       <c r="AM38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AN38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AO38" t="s">
         <v>55</v>
       </c>
       <c r="AP38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AA39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH39">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="AI39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ39">
         <v>2</v>
@@ -5602,28 +5487,28 @@
         <v>48</v>
       </c>
       <c r="AL39">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AM39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AN39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AO39" t="s">
         <v>56</v>
       </c>
       <c r="AP39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AA40" s="2"/>
       <c r="AH40">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="AI40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ40">
         <v>3</v>
@@ -5635,24 +5520,24 @@
         <v>30</v>
       </c>
       <c r="AM40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AN40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AO40" t="s">
         <v>19</v>
       </c>
       <c r="AP40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AH41">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="AI41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ41">
         <v>4</v>
@@ -5664,53 +5549,53 @@
         <v>10</v>
       </c>
       <c r="AM41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AN41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AO41" t="s">
         <v>19</v>
       </c>
       <c r="AP41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AH42">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="AI42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ42">
         <v>5</v>
       </c>
       <c r="AK42">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AL42">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AM42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AN42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AO42" t="s">
         <v>55</v>
       </c>
       <c r="AP42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AH43">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="AI43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ43">
         <v>6</v>
@@ -5722,45 +5607,45 @@
         <v>44</v>
       </c>
       <c r="AM43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AN43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AO43" t="s">
         <v>22</v>
       </c>
       <c r="AP43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AH44">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="AI44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AJ44">
         <v>7</v>
       </c>
       <c r="AK44">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="AL44">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AM44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AN44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AO44" t="s">
         <v>24</v>
       </c>
       <c r="AP44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed json for puckjs
</commit_message>
<xml_diff>
--- a/documentation/Map.xlsx
+++ b/documentation/Map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="125">
   <si>
     <t>ID</t>
   </si>
@@ -3787,15 +3787,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>17931</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>170889</xdr:rowOff>
+      <xdr:colOff>6725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>2800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>187431</xdr:colOff>
+      <xdr:colOff>176225</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>149889</xdr:rowOff>
+      <xdr:rowOff>172300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3804,7 +3804,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4679578" y="2837889"/>
+          <a:off x="4668372" y="2860300"/>
           <a:ext cx="360000" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3835,6 +3835,128 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>31937</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>17928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>10937</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>187428</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Ellipse 58"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2407584" y="1922928"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>4</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>82923</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>22972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>61923</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1972</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Ellipse 68"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2077570" y="1927972"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="42BA06"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>6</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4265,7 +4387,7 @@
         <v>2</v>
       </c>
       <c r="AK4">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AL4">
         <v>3</v>
@@ -4399,7 +4521,7 @@
         <v>6</v>
       </c>
       <c r="AK8">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AL8">
         <v>3</v>
@@ -4498,7 +4620,7 @@
         <v>1</v>
       </c>
       <c r="AK11">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AL11">
         <v>3</v>
@@ -4600,7 +4722,7 @@
         <v>1</v>
       </c>
       <c r="AK14">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AL14">
         <v>10</v>
@@ -4667,7 +4789,7 @@
         <v>0</v>
       </c>
       <c r="AK16">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AL16">
         <v>3</v>
@@ -4833,7 +4955,7 @@
         <v>0</v>
       </c>
       <c r="AK21">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AL21">
         <v>10</v>
@@ -5021,8 +5143,8 @@
       <c r="AB27">
         <v>27</v>
       </c>
-      <c r="AH27" t="s">
-        <v>106</v>
+      <c r="AH27">
+        <v>24</v>
       </c>
       <c r="AI27" t="s">
         <v>34</v>
@@ -5030,6 +5152,12 @@
       <c r="AJ27">
         <v>6</v>
       </c>
+      <c r="AK27">
+        <v>70</v>
+      </c>
+      <c r="AL27">
+        <v>58</v>
+      </c>
       <c r="AM27" t="s">
         <v>61</v>
       </c>
@@ -5040,7 +5168,7 @@
         <v>55</v>
       </c>
       <c r="AP27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="28:42" x14ac:dyDescent="0.25">
@@ -5048,7 +5176,7 @@
         <v>24</v>
       </c>
       <c r="AH28">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AI28" t="s">
         <v>35</v>
@@ -5080,7 +5208,7 @@
         <v>21</v>
       </c>
       <c r="AH29">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AI29" t="s">
         <v>35</v>
@@ -5112,7 +5240,7 @@
         <v>18</v>
       </c>
       <c r="AH30">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AI30" t="s">
         <v>35</v>
@@ -5144,7 +5272,7 @@
         <v>15</v>
       </c>
       <c r="AH31">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AI31" t="s">
         <v>35</v>
@@ -5175,8 +5303,8 @@
       <c r="AB32">
         <v>12</v>
       </c>
-      <c r="AH32" t="s">
-        <v>106</v>
+      <c r="AH32">
+        <v>29</v>
       </c>
       <c r="AI32" t="s">
         <v>35</v>
@@ -5184,6 +5312,12 @@
       <c r="AJ32">
         <v>4</v>
       </c>
+      <c r="AK32">
+        <v>70</v>
+      </c>
+      <c r="AL32">
+        <v>51</v>
+      </c>
       <c r="AM32" t="s">
         <v>66</v>
       </c>
@@ -5194,7 +5328,7 @@
         <v>55</v>
       </c>
       <c r="AP32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:42" x14ac:dyDescent="0.25">
@@ -5202,7 +5336,7 @@
         <v>10</v>
       </c>
       <c r="AH33">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AI33" t="s">
         <v>36</v>
@@ -5234,7 +5368,7 @@
         <v>8</v>
       </c>
       <c r="AH34">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AI34" t="s">
         <v>36</v>
@@ -5266,7 +5400,7 @@
         <v>5</v>
       </c>
       <c r="AH35">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AI35" t="s">
         <v>45</v>
@@ -5298,7 +5432,7 @@
         <v>2</v>
       </c>
       <c r="AH36">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AI36" t="s">
         <v>38</v>
@@ -5307,7 +5441,7 @@
         <v>0</v>
       </c>
       <c r="AK36">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AL36">
         <v>17</v>
@@ -5333,7 +5467,7 @@
         <v>98</v>
       </c>
       <c r="AH37">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AI37" t="s">
         <v>107</v>
@@ -5443,7 +5577,7 @@
         <v>0</v>
       </c>
       <c r="AH38">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AI38" t="s">
         <v>107</v>
@@ -5475,7 +5609,7 @@
         <v>99</v>
       </c>
       <c r="AH39">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AI39" t="s">
         <v>107</v>
@@ -5505,7 +5639,7 @@
     <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AA40" s="2"/>
       <c r="AH40">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AI40" t="s">
         <v>107</v>
@@ -5534,7 +5668,7 @@
     </row>
     <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AH41">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AI41" t="s">
         <v>107</v>
@@ -5563,7 +5697,7 @@
     </row>
     <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AH42">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AI42" t="s">
         <v>107</v>
@@ -5592,7 +5726,7 @@
     </row>
     <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AH43">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AI43" t="s">
         <v>107</v>
@@ -5621,7 +5755,7 @@
     </row>
     <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AH44">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AI44" t="s">
         <v>107</v>

</xml_diff>